<commit_message>
Create ExcelCreator with saving data to sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F6D7D0C-3ADE-42AF-8820-7C0E73DB1547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanin\IdeaProjects\vlad-laba\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA6CE7-EA08-4010-879E-63F1AADD9542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Отчет о работе с обучающимися с приминением дистанционных образовательных технологий</t>
   </si>
@@ -62,7 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -211,9 +217,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -226,21 +236,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -458,11 +464,11 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
@@ -471,83 +477,83 @@
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" ht="12.75">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="13"/>
       <c r="D5" s="14"/>
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="12.75">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -563,4 +569,118 @@
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC4C9F6-BB1D-40BD-A400-C60E44E071F6}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:D6"/>
+    <mergeCell ref="E4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+  </mergeCells>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+</worksheet>
 </file>
</xml_diff>